<commit_message>
Trabajo completo de backend
</commit_message>
<xml_diff>
--- a/backend/datos.xlsx
+++ b/backend/datos.xlsx
@@ -1,80 +1,122 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Semestre actual\Metodologías de desarrollo de software\Unidad 2.2\Prueba\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Semestre actual\Metodologías de desarrollo de software\Unidad 2.2\Metodologias-de-desarrollo-de-software-UPB\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29FB57D-9BE4-46B9-8631-7407710344B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B95C5D2-07DC-47F1-B84F-A2DE43A1486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="productos" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Los miamis</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Rionegro</t>
-  </si>
-  <si>
-    <t>Número de documento</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>4321</t>
-  </si>
-  <si>
-    <t>3333</t>
-  </si>
-  <si>
-    <t>Juli</t>
-  </si>
-  <si>
-    <t>3115678901</t>
-  </si>
-  <si>
-    <t>Medellin</t>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>Coca-cola</t>
+  </si>
+  <si>
+    <t>2.000</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Manzana</t>
+  </si>
+  <si>
+    <t>Uva</t>
+  </si>
+  <si>
+    <t>3.000</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>Naranja</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Bretaña</t>
+  </si>
+  <si>
+    <t>1.500</t>
+  </si>
+  <si>
+    <t>2.500</t>
+  </si>
+  <si>
+    <t>4.000</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,80 +427,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3118815062</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
-        <v>3174604014</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>